<commit_message>
Alteration of mini heatmaps and addition of class I-VI heatmaps
</commit_message>
<xml_diff>
--- a/CF39vsCF39S/Pure Temperature Analysis Comparisons/Individual Heatmaps/Raw Individual Segments of big heatmap.xlsx
+++ b/CF39vsCF39S/Pure Temperature Analysis Comparisons/Individual Heatmaps/Raw Individual Segments of big heatmap.xlsx
@@ -9,11 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20505" windowHeight="10350"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20505" windowHeight="10350" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Phage cluster 2" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Class 2 Heat Map" sheetId="2" r:id="rId2"/>
+    <sheet name="Class 3 Heat Map" sheetId="3" r:id="rId3"/>
+    <sheet name="Class 5 Heat Map" sheetId="4" r:id="rId4"/>
+    <sheet name="Class 6 Heat Map" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="102">
   <si>
     <t>locus</t>
   </si>
@@ -145,6 +148,193 @@
   </si>
   <si>
     <t>PROKKA_06417_sense</t>
+  </si>
+  <si>
+    <t>PROKKA_01964_sense</t>
+  </si>
+  <si>
+    <t>PROKKA_01965_sense</t>
+  </si>
+  <si>
+    <t>PROKKA_01967_sense</t>
+  </si>
+  <si>
+    <t>PROKKA_01968_sense</t>
+  </si>
+  <si>
+    <t>PROKKA_01970_sense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SuspectedProtein
+</t>
+  </si>
+  <si>
+    <t>pelA</t>
+  </si>
+  <si>
+    <t>pelB</t>
+  </si>
+  <si>
+    <t>pelD</t>
+  </si>
+  <si>
+    <t>pelE</t>
+  </si>
+  <si>
+    <t>pelG</t>
+  </si>
+  <si>
+    <t>PROKKA_05336_sense</t>
+  </si>
+  <si>
+    <t>PROKKA_05337_sense</t>
+  </si>
+  <si>
+    <t>cdrB</t>
+  </si>
+  <si>
+    <t>cdrA</t>
+  </si>
+  <si>
+    <t>PROKKA_00699_antis</t>
+  </si>
+  <si>
+    <t>rpsJ</t>
+  </si>
+  <si>
+    <t>PROKKA_00696_antis</t>
+  </si>
+  <si>
+    <t>rpsG</t>
+  </si>
+  <si>
+    <t>PROKKA_01423_sense</t>
+  </si>
+  <si>
+    <t>rpmE2</t>
+  </si>
+  <si>
+    <t>PROKKA_01285_sense</t>
+  </si>
+  <si>
+    <t>PROKKA_06065_antis</t>
+  </si>
+  <si>
+    <t>rpmB</t>
+  </si>
+  <si>
+    <t>PROKKA_04963_antis</t>
+  </si>
+  <si>
+    <t>groEL</t>
+  </si>
+  <si>
+    <t>PROKKA_00700_antis</t>
+  </si>
+  <si>
+    <t>PROKKA_00705_antis</t>
+  </si>
+  <si>
+    <t>rplC</t>
+  </si>
+  <si>
+    <t>rplV</t>
+  </si>
+  <si>
+    <t>PROKKA_00697_antis</t>
+  </si>
+  <si>
+    <t>fusA1</t>
+  </si>
+  <si>
+    <t>PROKKA_03630_sense</t>
+  </si>
+  <si>
+    <t>tRNA-Leu</t>
+  </si>
+  <si>
+    <t>PROKKA_00684_sense</t>
+  </si>
+  <si>
+    <t>secE</t>
+  </si>
+  <si>
+    <t>PROKKA_00821_sense</t>
+  </si>
+  <si>
+    <t>PROKKA_00823_sense</t>
+  </si>
+  <si>
+    <t>PROKKA_03624_antis</t>
+  </si>
+  <si>
+    <t>PROKKA_03625_antis</t>
+  </si>
+  <si>
+    <t>parR</t>
+  </si>
+  <si>
+    <t>parS</t>
+  </si>
+  <si>
+    <t>PROKKA_04456_sense</t>
+  </si>
+  <si>
+    <t>cupC2</t>
+  </si>
+  <si>
+    <t>PROKKA_02566_antis</t>
+  </si>
+  <si>
+    <t>PROKKA_02612_antis</t>
+  </si>
+  <si>
+    <t>PROKKA_02613_antis</t>
+  </si>
+  <si>
+    <t>SuspectedProtein</t>
+  </si>
+  <si>
+    <t>PROKKA_00087_sense</t>
+  </si>
+  <si>
+    <t>tssA1</t>
+  </si>
+  <si>
+    <t>PROKKA_00089_sense</t>
+  </si>
+  <si>
+    <t>tssC1</t>
+  </si>
+  <si>
+    <t>PROKKA_00090_sense</t>
+  </si>
+  <si>
+    <t>hcp1</t>
+  </si>
+  <si>
+    <t>PROKKA_00095_sense</t>
+  </si>
+  <si>
+    <t>clpV1</t>
+  </si>
+  <si>
+    <t>PROKKA_05793_sense</t>
+  </si>
+  <si>
+    <t>HslV</t>
+  </si>
+  <si>
+    <t>PROKKA_05794_sense</t>
+  </si>
+  <si>
+    <t>HslU</t>
+  </si>
+  <si>
+    <t>PROKKA_00088_sense</t>
+  </si>
+  <si>
+    <t>tssB1</t>
   </si>
 </sst>
 </file>
@@ -192,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -200,6 +390,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1175,12 +1373,910 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2">
+        <v>3.7199824531975221</v>
+      </c>
+      <c r="E2">
+        <v>3.5169113041071087</v>
+      </c>
+      <c r="F2">
+        <v>3.636072112353522</v>
+      </c>
+      <c r="G2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3">
+        <v>3.6572182483515636</v>
+      </c>
+      <c r="E3">
+        <v>3.2090297022852177</v>
+      </c>
+      <c r="F3">
+        <v>2.7997425569531091</v>
+      </c>
+      <c r="G3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4">
+        <v>5.7919215723062782</v>
+      </c>
+      <c r="F4">
+        <v>5.1220279413740259</v>
+      </c>
+      <c r="G4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5">
+        <v>2.9350734993412724</v>
+      </c>
+      <c r="F5">
+        <v>3.2803152011888503</v>
+      </c>
+      <c r="G5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6">
+        <v>2.3719708361083063</v>
+      </c>
+      <c r="D6">
+        <v>2.9949594628171545</v>
+      </c>
+      <c r="E6">
+        <v>3.3718641064839354</v>
+      </c>
+      <c r="F6">
+        <v>3.4514459001269371</v>
+      </c>
+      <c r="G6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7">
+        <v>3.4708669769290998</v>
+      </c>
+      <c r="E7">
+        <v>3.8939757355084907</v>
+      </c>
+      <c r="F7">
+        <v>3.6305230173344087</v>
+      </c>
+      <c r="G7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8">
+        <v>2.0354002313364283</v>
+      </c>
+      <c r="D8">
+        <v>4.3908397915150106</v>
+      </c>
+      <c r="E8">
+        <v>3.1506046363855815</v>
+      </c>
+      <c r="F8">
+        <v>3.7560209774529683</v>
+      </c>
+      <c r="G8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2">
+        <v>2.9811517434244461</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3">
+        <v>2.7716738710072035</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4">
+        <v>2.6337272315076361</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4">
+        <v>2.4281923301386308</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3.372073877241327</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6">
+        <v>2.4685589053201422</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7">
+        <v>3.4083567151990031</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8">
+        <v>2.8830198992488394</v>
+      </c>
+      <c r="F8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9">
+        <v>3.0863058061575916</v>
+      </c>
+      <c r="F9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10">
+        <v>3.0980816644183506</v>
+      </c>
+      <c r="F10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11">
+        <v>1.8940071153403615</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12">
+        <v>2.5487880719145171</v>
+      </c>
+      <c r="F12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13">
+        <v>4.1689085617859067</v>
+      </c>
+      <c r="E13">
+        <v>2.1082380133680689</v>
+      </c>
+      <c r="F13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14">
+        <v>3.6403833847753573</v>
+      </c>
+      <c r="E14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2">
+        <v>-31.156138967172925</v>
+      </c>
+      <c r="C2">
+        <v>-6.0075766154898389</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3">
+        <v>-10.257376751860207</v>
+      </c>
+      <c r="C3">
+        <v>-10.106539816993013</v>
+      </c>
+      <c r="D3">
+        <v>-18.587278893252918</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4">
+        <v>-5.0960224413827291</v>
+      </c>
+      <c r="C4">
+        <v>-3.2216223892336409</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5">
+        <v>-6.6657437054992075</v>
+      </c>
+      <c r="C5">
+        <v>-7.8159789392448653</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6">
+        <v>-8.4607792664326098</v>
+      </c>
+      <c r="C6">
+        <v>-9.1804860839128857</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7">
+        <v>-12.838900285800088</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="A1:G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="6">
+        <v>-2.1307327690469124</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1.8922026508731662</v>
+      </c>
+      <c r="F2" s="6">
+        <v>2.3026647981748942</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6">
+        <v>-2.2113963336418321</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="6">
+        <v>2.0095193825812085</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="6">
+        <v>-1.884527605151143</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="6">
+        <v>2.165097821572759</v>
+      </c>
+      <c r="F4" s="6">
+        <v>2.0132088462653983</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="6">
+        <v>2.4919797765040346</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="6">
+        <v>2.0458105977734329</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="6">
+        <v>3.8995685999865501</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="6">
+        <v>5.3102654012313604</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>